<commit_message>
Products adding normal & detailed implemented
</commit_message>
<xml_diff>
--- a/public/fileStore/import_template/products_import_template.xlsx
+++ b/public/fileStore/import_template/products_import_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Little Pro\Desktop\APOTEk\APOTEK_SYSTEMS_POS\public\fileStore\import_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Little Pro\Desktop\APOTEk\apotek_systems_pos\public\fileStore\import_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23702E03-DA2A-48DE-B196-877101F77BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5585BEA9-7681-43F8-A562-7E84AB22B2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E4D20C7-D269-441D-A8EC-D6C44E917C10}"/>
   </bookViews>
@@ -22,17 +22,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Barcode</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Unit</t>
+    <t>Mo cola</t>
+  </si>
+  <si>
+    <t>BEVERAGE</t>
+  </si>
+  <si>
+    <t>ml</t>
   </si>
   <si>
     <r>
-      <t>Product Name</t>
+      <t>product_name</t>
     </r>
     <r>
       <rPr>
@@ -47,21 +47,7 @@
   </si>
   <si>
     <r>
-      <t>Product Code</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Category</t>
+      <t>category</t>
     </r>
     <r>
       <rPr>
@@ -75,22 +61,36 @@
     </r>
   </si>
   <si>
-    <t>Mo cola</t>
-  </si>
-  <si>
-    <t>BEVERAGE</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>Min Stock</t>
-  </si>
-  <si>
-    <t>Max Stock</t>
-  </si>
-  <si>
-    <t>Pack Size</t>
+    <t>pack_size</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>min_stock</t>
+  </si>
+  <si>
+    <t>max_stock</t>
+  </si>
+  <si>
+    <r>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -948,7 +948,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,25 +965,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -994,19 +994,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>102048</v>
+        <v>100001</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>300</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>